<commit_message>
Esecuzione test: [57, 157]
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CBSISTEMIXX/CB_Sistemi/StudioLAB/3.3.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111CBSISTEMIXX/CB_Sistemi/StudioLAB/3.3.0.0/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luca.lanzano\Desktop\FSE 2.0\Fork\it-fse-accreditamento\GATEWAY\A1#111CBSISTEMIXX\CB_Sistemi\StudioLAB\3.3.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B16D3B-9A77-422B-B255-16709557EEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EBBF6A-E25D-4670-B227-C0C013DDD15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="587">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1592,15 +1592,6 @@
     <t>Il documento sembra contenere valori non ammessi. Si prega di verificare.</t>
   </si>
   <si>
-    <t>2024-05-21T13:09:30Z</t>
-  </si>
-  <si>
-    <t>ee14288b68d64e21</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.46a41df0ab0514f11c0811056832c3225e06c8e11824f27c7e5517ca5cfc57fe.c033c9bf33^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2024-05-21T13:16:19Z</t>
   </si>
   <si>
@@ -2262,6 +2253,30 @@
   </si>
   <si>
     <t>Il software gestisce il campo della tipologia di accesso ma se il valore non corrisponde ai valori gestiti il tag NON viene inserito nel CDA2.</t>
+  </si>
+  <si>
+    <t>2024-07-16T09:32:19Z</t>
+  </si>
+  <si>
+    <t>23320df0b526a5e4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.2f09a51ca4cd16d36c3cccd566b5db9a2f5d03ba85357646ca5ec354e215e8e6.b4fb37e82f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Errore semantico. [ERRORE-33a| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR' ]</t>
+  </si>
+  <si>
+    <t>2024-07-16T09:46:20Z</t>
+  </si>
+  <si>
+    <t>7586e6c649f7b78f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.63fc3e871b635843f2dd0a7b1d3f0f53ad2420c7ccfd4e04415def543adf2965.ac00e55bec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>L’errore è registrato in un log applicativo. L’operatore (medico refertatore) ha 2 opzioni: A) provare a correggere l’errore sul campo sesso del paziente, richiedendo anche supporto al backoffice, e quindi generare un nuovo referto PDF da sottoporre al servizio di validazione. B) firmare digitalmente il referto PDF privo della validazione da parte del Gateway del CDA2 così da poter consegnare al paziente il referto. I referti PDF digitalmente firmati ma privi di validazione del CDA2, che non potranno essere pubblicati sul FSE, sono evidenziati in un pannello di servizio al medico refertatore in modo che possa procedere alla produzione, per il caso in oggetto,  di un nuovo referto PDF, riprocessandolo con validazione e firma digitale, dopo le correzioni necessarie.</t>
   </si>
 </sst>
 </file>
@@ -5232,7 +5247,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E68" sqref="E68"/>
+      <selection pane="bottomRight" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5737,13 +5752,13 @@
         <v>45456</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>83</v>
@@ -5787,7 +5802,7 @@
         <v>304</v>
       </c>
       <c r="K16" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
@@ -5825,7 +5840,7 @@
         <v>304</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
@@ -5863,7 +5878,7 @@
         <v>304</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
@@ -5922,7 +5937,7 @@
         <v>83</v>
       </c>
       <c r="P19" s="34" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="Q19" s="34" t="s">
         <v>302</v>
@@ -5955,10 +5970,10 @@
         <v>45456</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="I20" s="24" t="s">
         <v>327</v>
@@ -5974,13 +5989,13 @@
         <v>83</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="O20" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P20" s="25" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="Q20" s="25" t="s">
         <v>302</v>
@@ -6011,10 +6026,10 @@
         <v>45467</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I21" s="24" t="s">
         <v>327</v>
@@ -6030,13 +6045,13 @@
         <v>83</v>
       </c>
       <c r="N21" s="25" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="O21" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P21" s="25" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="Q21" s="25" t="s">
         <v>302</v>
@@ -6092,7 +6107,7 @@
         <v>83</v>
       </c>
       <c r="P22" s="34" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="Q22" s="34" t="s">
         <v>302</v>
@@ -6125,10 +6140,10 @@
         <v>45456</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="I23" s="24" t="s">
         <v>327</v>
@@ -6144,13 +6159,13 @@
         <v>83</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="O23" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P23" s="25" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="Q23" s="25" t="s">
         <v>302</v>
@@ -6181,10 +6196,10 @@
         <v>45467</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="I24" s="24" t="s">
         <v>327</v>
@@ -6200,13 +6215,13 @@
         <v>83</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="O24" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P24" s="25" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="Q24" s="25" t="s">
         <v>302</v>
@@ -6300,13 +6315,13 @@
         <v>83</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="O26" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P26" s="25" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="Q26" s="25" t="s">
         <v>302</v>
@@ -6350,13 +6365,13 @@
         <v>83</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="O27" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P27" s="25" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="Q27" s="25" t="s">
         <v>302</v>
@@ -6414,7 +6429,7 @@
         <v>83</v>
       </c>
       <c r="P28" s="34" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="Q28" s="34" t="s">
         <v>302</v>
@@ -6470,7 +6485,7 @@
         <v>83</v>
       </c>
       <c r="P29" s="34" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="Q29" s="34" t="s">
         <v>302</v>
@@ -6526,7 +6541,7 @@
         <v>83</v>
       </c>
       <c r="P30" s="34" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="Q30" s="34" t="s">
         <v>302</v>
@@ -6582,7 +6597,7 @@
         <v>83</v>
       </c>
       <c r="P31" s="34" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="Q31" s="34" t="s">
         <v>302</v>
@@ -6638,7 +6653,7 @@
         <v>83</v>
       </c>
       <c r="P32" s="34" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="Q32" s="34" t="s">
         <v>302</v>
@@ -6666,16 +6681,16 @@
         <v>97</v>
       </c>
       <c r="F33" s="23">
-        <v>45433</v>
+        <v>45489</v>
       </c>
       <c r="G33" s="35" t="s">
-        <v>358</v>
+        <v>583</v>
       </c>
       <c r="H33" s="35" t="s">
-        <v>359</v>
+        <v>584</v>
       </c>
       <c r="I33" s="35" t="s">
-        <v>360</v>
+        <v>585</v>
       </c>
       <c r="J33" s="34" t="s">
         <v>83</v>
@@ -6688,13 +6703,13 @@
         <v>83</v>
       </c>
       <c r="N33" s="34" t="s">
-        <v>357</v>
+        <v>479</v>
       </c>
       <c r="O33" s="34" t="s">
         <v>83</v>
       </c>
       <c r="P33" s="34" t="s">
-        <v>563</v>
+        <v>586</v>
       </c>
       <c r="Q33" s="34" t="s">
         <v>302</v>
@@ -6725,13 +6740,13 @@
         <v>45433</v>
       </c>
       <c r="G34" s="35" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="H34" s="35" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="I34" s="35" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="J34" s="34" t="s">
         <v>83</v>
@@ -6750,7 +6765,7 @@
         <v>83</v>
       </c>
       <c r="P34" s="34" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="Q34" s="34" t="s">
         <v>302</v>
@@ -6781,13 +6796,13 @@
         <v>45433</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="H35" s="35" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="I35" s="35" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="J35" s="34" t="s">
         <v>83</v>
@@ -6800,13 +6815,13 @@
         <v>83</v>
       </c>
       <c r="N35" s="34" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="O35" s="34" t="s">
         <v>83</v>
       </c>
       <c r="P35" s="34" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="Q35" s="34" t="s">
         <v>302</v>
@@ -6837,13 +6852,13 @@
         <v>45433</v>
       </c>
       <c r="G36" s="35" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H36" s="35" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I36" s="35" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="J36" s="34" t="s">
         <v>83</v>
@@ -6862,7 +6877,7 @@
         <v>83</v>
       </c>
       <c r="P36" s="34" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="Q36" s="34" t="s">
         <v>302</v>
@@ -6893,13 +6908,13 @@
         <v>45433</v>
       </c>
       <c r="G37" s="35" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="H37" s="35" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="I37" s="35" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="J37" s="34" t="s">
         <v>83</v>
@@ -6912,13 +6927,13 @@
         <v>83</v>
       </c>
       <c r="N37" s="34" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="O37" s="34" t="s">
         <v>83</v>
       </c>
       <c r="P37" s="34" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="Q37" s="34" t="s">
         <v>302</v>
@@ -6949,13 +6964,13 @@
         <v>45433</v>
       </c>
       <c r="G38" s="35" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="H38" s="35" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="I38" s="35" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="J38" s="34" t="s">
         <v>83</v>
@@ -6968,13 +6983,13 @@
         <v>83</v>
       </c>
       <c r="N38" s="34" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="O38" s="34" t="s">
         <v>83</v>
       </c>
       <c r="P38" s="34" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="Q38" s="34" t="s">
         <v>302</v>
@@ -7005,13 +7020,13 @@
         <v>45456</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="I39" s="24" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="J39" s="25" t="s">
         <v>83</v>
@@ -7024,13 +7039,13 @@
         <v>83</v>
       </c>
       <c r="N39" s="25" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="O39" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P39" s="25" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="Q39" s="25" t="s">
         <v>302</v>
@@ -7061,13 +7076,13 @@
         <v>45456</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="H40" s="24" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="J40" s="25" t="s">
         <v>83</v>
@@ -7080,13 +7095,13 @@
         <v>83</v>
       </c>
       <c r="N40" s="25" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="O40" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P40" s="25" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="Q40" s="25" t="s">
         <v>302</v>
@@ -7117,13 +7132,13 @@
         <v>45456</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>83</v>
@@ -7136,13 +7151,13 @@
         <v>83</v>
       </c>
       <c r="N41" s="25" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="O41" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P41" s="25" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="Q41" s="25" t="s">
         <v>302</v>
@@ -7173,13 +7188,13 @@
         <v>45456</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H42" s="24" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="I42" s="24" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="J42" s="25" t="s">
         <v>83</v>
@@ -7192,13 +7207,13 @@
         <v>83</v>
       </c>
       <c r="N42" s="25" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="O42" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P42" s="25" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="Q42" s="25" t="s">
         <v>302</v>
@@ -7229,13 +7244,13 @@
         <v>45456</v>
       </c>
       <c r="G43" s="24" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="J43" s="25" t="s">
         <v>83</v>
@@ -7248,13 +7263,13 @@
         <v>83</v>
       </c>
       <c r="N43" s="25" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="O43" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P43" s="25" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="Q43" s="25" t="s">
         <v>302</v>
@@ -7285,13 +7300,13 @@
         <v>45456</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I44" s="24" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="J44" s="25" t="s">
         <v>83</v>
@@ -7304,13 +7319,13 @@
         <v>83</v>
       </c>
       <c r="N44" s="25" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="O44" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P44" s="25" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="Q44" s="25" t="s">
         <v>302</v>
@@ -7345,7 +7360,7 @@
         <v>304</v>
       </c>
       <c r="K45" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L45" s="25"/>
       <c r="M45" s="25"/>
@@ -7379,13 +7394,13 @@
         <v>45464</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>83</v>
@@ -7398,13 +7413,13 @@
         <v>83</v>
       </c>
       <c r="N46" s="25" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="O46" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P46" s="34" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="Q46" s="25" t="s">
         <v>302</v>
@@ -7435,13 +7450,13 @@
         <v>45464</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>83</v>
@@ -7454,13 +7469,13 @@
         <v>83</v>
       </c>
       <c r="N47" s="25" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="O47" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P47" s="34" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="Q47" s="25" t="s">
         <v>302</v>
@@ -7491,13 +7506,13 @@
         <v>45464</v>
       </c>
       <c r="G48" s="35" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="H48" s="35" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="I48" s="35" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="J48" s="34" t="s">
         <v>83</v>
@@ -7510,13 +7525,13 @@
         <v>83</v>
       </c>
       <c r="N48" s="34" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="O48" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P48" s="34" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="Q48" s="25" t="s">
         <v>302</v>
@@ -7547,13 +7562,13 @@
         <v>45464</v>
       </c>
       <c r="G49" s="35" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="H49" s="35" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="I49" s="35" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="J49" s="25" t="s">
         <v>83</v>
@@ -7566,13 +7581,13 @@
         <v>83</v>
       </c>
       <c r="N49" s="34" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="O49" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P49" s="34" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="Q49" s="25" t="s">
         <v>302</v>
@@ -7607,7 +7622,7 @@
         <v>304</v>
       </c>
       <c r="K50" s="34" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L50" s="25"/>
       <c r="M50" s="25"/>
@@ -7645,7 +7660,7 @@
         <v>304</v>
       </c>
       <c r="K51" s="34" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L51" s="25"/>
       <c r="M51" s="25"/>
@@ -7683,7 +7698,7 @@
         <v>304</v>
       </c>
       <c r="K52" s="34" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L52" s="25"/>
       <c r="M52" s="25"/>
@@ -7721,7 +7736,7 @@
         <v>304</v>
       </c>
       <c r="K53" s="34" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L53" s="25"/>
       <c r="M53" s="25"/>
@@ -7759,7 +7774,7 @@
         <v>304</v>
       </c>
       <c r="K54" s="34" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L54" s="25"/>
       <c r="M54" s="25"/>
@@ -7797,7 +7812,7 @@
         <v>304</v>
       </c>
       <c r="K55" s="34" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
@@ -7835,7 +7850,7 @@
         <v>304</v>
       </c>
       <c r="K56" s="34" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L56" s="25"/>
       <c r="M56" s="25"/>
@@ -7869,13 +7884,13 @@
         <v>45467</v>
       </c>
       <c r="G57" s="35" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="H57" s="35" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="I57" s="35" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="J57" s="25" t="s">
         <v>83</v>
@@ -7888,13 +7903,13 @@
         <v>83</v>
       </c>
       <c r="N57" s="41" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="O57" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P57" s="34" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="Q57" s="25" t="s">
         <v>302</v>
@@ -7929,7 +7944,7 @@
         <v>304</v>
       </c>
       <c r="K58" s="25" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="L58" s="25"/>
       <c r="M58" s="25"/>
@@ -7967,7 +7982,7 @@
         <v>304</v>
       </c>
       <c r="K59" s="25" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="L59" s="25"/>
       <c r="M59" s="25"/>
@@ -8005,7 +8020,7 @@
         <v>304</v>
       </c>
       <c r="K60" s="25" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="L60" s="25"/>
       <c r="M60" s="25"/>
@@ -8043,7 +8058,7 @@
         <v>304</v>
       </c>
       <c r="K61" s="25" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="L61" s="25"/>
       <c r="M61" s="25"/>
@@ -8077,13 +8092,13 @@
         <v>45467</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H62" s="24" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="J62" s="25" t="s">
         <v>83</v>
@@ -8096,13 +8111,13 @@
         <v>83</v>
       </c>
       <c r="N62" s="25" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="O62" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P62" s="25" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="Q62" s="25" t="s">
         <v>302</v>
@@ -8133,13 +8148,13 @@
         <v>45467</v>
       </c>
       <c r="G63" s="24" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="H63" s="24" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I63" s="24" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="J63" s="25" t="s">
         <v>83</v>
@@ -8152,13 +8167,13 @@
         <v>83</v>
       </c>
       <c r="N63" s="25" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="O63" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P63" s="25" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="Q63" s="25" t="s">
         <v>302</v>
@@ -8189,13 +8204,13 @@
         <v>45467</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="H64" s="24" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="I64" s="24" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="J64" s="25" t="s">
         <v>83</v>
@@ -8208,13 +8223,13 @@
         <v>83</v>
       </c>
       <c r="N64" s="25" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="O64" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P64" s="25" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="Q64" s="25" t="s">
         <v>302</v>
@@ -8245,13 +8260,13 @@
         <v>45467</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H65" s="24" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="J65" s="25" t="s">
         <v>83</v>
@@ -8264,13 +8279,13 @@
         <v>83</v>
       </c>
       <c r="N65" s="25" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="O65" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P65" s="25" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="Q65" s="25" t="s">
         <v>302</v>
@@ -8301,13 +8316,13 @@
         <v>45467</v>
       </c>
       <c r="G66" s="24" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="H66" s="24" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="I66" s="24" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="J66" s="25" t="s">
         <v>83</v>
@@ -8320,13 +8335,13 @@
         <v>83</v>
       </c>
       <c r="N66" s="25" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="O66" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P66" s="25" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="Q66" s="25" t="s">
         <v>302</v>
@@ -8357,13 +8372,13 @@
         <v>45467</v>
       </c>
       <c r="G67" s="24" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="H67" s="24" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="I67" s="24" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="J67" s="25" t="s">
         <v>83</v>
@@ -8376,13 +8391,13 @@
         <v>83</v>
       </c>
       <c r="N67" s="25" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="O67" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P67" s="25" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="Q67" s="25" t="s">
         <v>302</v>
@@ -8393,7 +8408,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="20">
         <v>157</v>
       </c>
@@ -8409,21 +8424,39 @@
       <c r="E68" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="F68" s="23"/>
-      <c r="G68" s="24"/>
-      <c r="H68" s="24"/>
-      <c r="I68" s="24"/>
+      <c r="F68" s="23">
+        <v>45489</v>
+      </c>
+      <c r="G68" s="24" t="s">
+        <v>579</v>
+      </c>
+      <c r="H68" s="24" t="s">
+        <v>580</v>
+      </c>
+      <c r="I68" s="24" t="s">
+        <v>581</v>
+      </c>
       <c r="J68" s="25" t="s">
-        <v>304</v>
+        <v>83</v>
       </c>
       <c r="K68" s="25" t="s">
-        <v>581</v>
-      </c>
-      <c r="L68" s="27"/>
-      <c r="M68" s="27"/>
-      <c r="N68" s="25"/>
-      <c r="O68" s="27"/>
-      <c r="P68" s="25"/>
+        <v>578</v>
+      </c>
+      <c r="L68" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="M68" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="N68" s="25" t="s">
+        <v>582</v>
+      </c>
+      <c r="O68" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="P68" s="25" t="s">
+        <v>571</v>
+      </c>
       <c r="Q68" s="27"/>
       <c r="R68" s="26"/>
       <c r="S68" s="27"/>
@@ -8451,13 +8484,13 @@
         <v>45467</v>
       </c>
       <c r="G69" s="24" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="H69" s="24" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="I69" s="24" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="J69" s="25" t="s">
         <v>83</v>
@@ -8470,13 +8503,13 @@
         <v>83</v>
       </c>
       <c r="N69" s="25" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="O69" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P69" s="25" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="Q69" s="25" t="s">
         <v>302</v>
@@ -8507,13 +8540,13 @@
         <v>45467</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="H70" s="24" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="I70" s="24" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J70" s="25" t="s">
         <v>83</v>
@@ -8526,13 +8559,13 @@
         <v>83</v>
       </c>
       <c r="N70" s="25" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="O70" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P70" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="Q70" s="25" t="s">
         <v>302</v>
@@ -8563,13 +8596,13 @@
         <v>45467</v>
       </c>
       <c r="G71" s="24" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="H71" s="24" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="J71" s="25" t="s">
         <v>83</v>
@@ -8582,13 +8615,13 @@
         <v>83</v>
       </c>
       <c r="N71" s="25" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="O71" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P71" s="25" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="Q71" s="25" t="s">
         <v>302</v>
@@ -8619,13 +8652,13 @@
         <v>45468</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="J72" s="25" t="s">
         <v>83</v>
@@ -8638,13 +8671,13 @@
         <v>83</v>
       </c>
       <c r="N72" s="25" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="O72" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P72" s="25" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="Q72" s="25" t="s">
         <v>302</v>
@@ -8679,7 +8712,7 @@
         <v>304</v>
       </c>
       <c r="K73" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L73" s="25"/>
       <c r="M73" s="25"/>
@@ -8717,7 +8750,7 @@
         <v>304</v>
       </c>
       <c r="K74" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L74" s="25"/>
       <c r="M74" s="25"/>
@@ -8755,7 +8788,7 @@
         <v>304</v>
       </c>
       <c r="K75" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L75" s="25"/>
       <c r="M75" s="25"/>
@@ -8793,7 +8826,7 @@
         <v>304</v>
       </c>
       <c r="K76" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L76" s="25"/>
       <c r="M76" s="25"/>
@@ -8831,7 +8864,7 @@
         <v>304</v>
       </c>
       <c r="K77" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L77" s="25"/>
       <c r="M77" s="25"/>
@@ -8869,7 +8902,7 @@
         <v>304</v>
       </c>
       <c r="K78" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L78" s="25"/>
       <c r="M78" s="25"/>
@@ -8907,7 +8940,7 @@
         <v>304</v>
       </c>
       <c r="K79" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L79" s="25"/>
       <c r="M79" s="25"/>
@@ -8941,13 +8974,13 @@
         <v>45468</v>
       </c>
       <c r="G80" s="24" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="H80" s="24" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="I80" s="24" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="J80" s="25" t="s">
         <v>83</v>
@@ -8960,13 +8993,13 @@
         <v>83</v>
       </c>
       <c r="N80" s="25" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="O80" s="25" t="s">
         <v>83</v>
       </c>
       <c r="P80" s="25" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="Q80" s="25" t="s">
         <v>302</v>
@@ -9001,7 +9034,7 @@
         <v>304</v>
       </c>
       <c r="K81" s="25" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="L81" s="25"/>
       <c r="M81" s="25"/>
@@ -9037,13 +9070,13 @@
         <v>45436</v>
       </c>
       <c r="G82" s="24" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H82" s="24" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="J82" s="25" t="s">
         <v>83</v>
@@ -9083,13 +9116,13 @@
         <v>45436</v>
       </c>
       <c r="G83" s="24" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H83" s="24" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I83" s="24" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="J83" s="25" t="s">
         <v>83</v>
@@ -9129,13 +9162,13 @@
         <v>45436</v>
       </c>
       <c r="G84" s="24" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="H84" s="24" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I84" s="24" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="J84" s="25" t="s">
         <v>83</v>
@@ -9175,13 +9208,13 @@
         <v>45436</v>
       </c>
       <c r="G85" s="24" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H85" s="24" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="I85" s="24" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="J85" s="25" t="s">
         <v>83</v>
@@ -9221,13 +9254,13 @@
         <v>45439</v>
       </c>
       <c r="G86" s="35" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="H86" s="35" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="I86" s="35" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="J86" s="34" t="s">
         <v>83</v>
@@ -9267,10 +9300,10 @@
         <v>45439</v>
       </c>
       <c r="G87" s="35" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H87" s="35" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="I87" s="35" t="s">
         <v>327</v>
@@ -9286,7 +9319,7 @@
         <v>83</v>
       </c>
       <c r="N87" s="34" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="O87" s="34" t="s">
         <v>83</v>
@@ -9323,10 +9356,10 @@
         <v>45439</v>
       </c>
       <c r="G88" s="35" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="H88" s="35" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I88" s="35" t="s">
         <v>327</v>
@@ -9342,7 +9375,7 @@
         <v>83</v>
       </c>
       <c r="N88" s="34" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="O88" s="34" t="s">
         <v>83</v>
@@ -9355,7 +9388,7 @@
       </c>
       <c r="R88" s="26"/>
       <c r="S88" s="40" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="T88" s="28" t="s">
         <v>72</v>
@@ -9381,13 +9414,13 @@
         <v>45439</v>
       </c>
       <c r="G89" s="35" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="H89" s="35" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I89" s="35" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="J89" s="34" t="s">
         <v>83</v>
@@ -9400,7 +9433,7 @@
         <v>83</v>
       </c>
       <c r="N89" s="34" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="O89" s="34" t="s">
         <v>83</v>
@@ -9437,10 +9470,10 @@
         <v>45439</v>
       </c>
       <c r="G90" s="35" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="H90" s="35" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="I90" s="35" t="s">
         <v>327</v>
@@ -9456,7 +9489,7 @@
         <v>83</v>
       </c>
       <c r="N90" s="34" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="O90" s="34" t="s">
         <v>83</v>
@@ -9493,13 +9526,13 @@
         <v>45439</v>
       </c>
       <c r="G91" s="35" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="H91" s="35" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I91" s="35" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="J91" s="34" t="s">
         <v>83</v>
@@ -9516,7 +9549,7 @@
         <v>83</v>
       </c>
       <c r="P91" s="34" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="Q91" s="34" t="s">
         <v>302</v>
@@ -9547,13 +9580,13 @@
         <v>45439</v>
       </c>
       <c r="G92" s="35" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H92" s="35" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I92" s="35" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="J92" s="34" t="s">
         <v>83</v>
@@ -9570,7 +9603,7 @@
         <v>83</v>
       </c>
       <c r="P92" s="34" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="Q92" s="34" t="s">
         <v>302</v>
@@ -9601,13 +9634,13 @@
         <v>45439</v>
       </c>
       <c r="G93" s="35" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H93" s="35" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I93" s="35" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="J93" s="34" t="s">
         <v>83</v>
@@ -9624,7 +9657,7 @@
         <v>83</v>
       </c>
       <c r="P93" s="34" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="Q93" s="34" t="s">
         <v>302</v>
@@ -9655,10 +9688,10 @@
         <v>45439</v>
       </c>
       <c r="G94" s="35" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H94" s="35" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="I94" s="35" t="s">
         <v>327</v>
@@ -9674,7 +9707,7 @@
         <v>83</v>
       </c>
       <c r="N94" s="34" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="O94" s="34" t="s">
         <v>83</v>
@@ -9711,10 +9744,10 @@
         <v>45439</v>
       </c>
       <c r="G95" s="35" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="H95" s="35" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="I95" s="35" t="s">
         <v>327</v>
@@ -9730,7 +9763,7 @@
         <v>83</v>
       </c>
       <c r="N95" s="34" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="O95" s="34" t="s">
         <v>83</v>
@@ -9767,10 +9800,10 @@
         <v>45446</v>
       </c>
       <c r="G96" s="24" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H96" s="24" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="I96" s="24" t="s">
         <v>327</v>
@@ -9786,7 +9819,7 @@
         <v>83</v>
       </c>
       <c r="N96" s="25" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="O96" s="25" t="s">
         <v>83</v>
@@ -9823,10 +9856,10 @@
         <v>45447</v>
       </c>
       <c r="G97" s="24" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="H97" s="24" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="I97" s="24" t="s">
         <v>327</v>
@@ -9842,7 +9875,7 @@
         <v>83</v>
       </c>
       <c r="N97" s="25" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="O97" s="25" t="s">
         <v>83</v>
@@ -9879,10 +9912,10 @@
         <v>45447</v>
       </c>
       <c r="G98" s="24" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="H98" s="24" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="I98" s="24" t="s">
         <v>327</v>
@@ -9898,7 +9931,7 @@
         <v>83</v>
       </c>
       <c r="N98" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="O98" s="25" t="s">
         <v>83</v>
@@ -9935,10 +9968,10 @@
         <v>45447</v>
       </c>
       <c r="G99" s="24" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="H99" s="24" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="I99" s="24" t="s">
         <v>327</v>
@@ -9954,7 +9987,7 @@
         <v>83</v>
       </c>
       <c r="N99" s="25" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="O99" s="25" t="s">
         <v>83</v>
@@ -9991,10 +10024,10 @@
         <v>45447</v>
       </c>
       <c r="G100" s="24" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H100" s="24" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I100" s="24" t="s">
         <v>327</v>
@@ -10010,7 +10043,7 @@
         <v>83</v>
       </c>
       <c r="N100" s="25" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="O100" s="25" t="s">
         <v>83</v>
@@ -10047,10 +10080,10 @@
         <v>45447</v>
       </c>
       <c r="G101" s="24" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="H101" s="24" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="I101" s="24" t="s">
         <v>327</v>
@@ -10066,7 +10099,7 @@
         <v>83</v>
       </c>
       <c r="N101" s="25" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="O101" s="25" t="s">
         <v>83</v>
@@ -10103,10 +10136,10 @@
         <v>45447</v>
       </c>
       <c r="G102" s="24" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H102" s="24" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="I102" s="24" t="s">
         <v>327</v>
@@ -10122,7 +10155,7 @@
         <v>83</v>
       </c>
       <c r="N102" s="25" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="O102" s="25" t="s">
         <v>83</v>
@@ -10159,10 +10192,10 @@
         <v>45447</v>
       </c>
       <c r="G103" s="24" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H103" s="24" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="I103" s="24" t="s">
         <v>327</v>
@@ -10178,7 +10211,7 @@
         <v>83</v>
       </c>
       <c r="N103" s="25" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="O103" s="25" t="s">
         <v>83</v>
@@ -10215,13 +10248,13 @@
         <v>45447</v>
       </c>
       <c r="G104" s="24" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H104" s="24" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="I104" s="24" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="J104" s="25" t="s">
         <v>83</v>
@@ -10261,13 +10294,13 @@
         <v>45467</v>
       </c>
       <c r="G105" s="35" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="H105" s="35" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="I105" s="35" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="J105" s="25" t="s">
         <v>83</v>
@@ -10307,13 +10340,13 @@
         <v>45468</v>
       </c>
       <c r="G106" s="24" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="H106" s="24" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="I106" s="24" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="J106" s="25" t="s">
         <v>83</v>
@@ -10357,7 +10390,7 @@
         <v>304</v>
       </c>
       <c r="K107" s="25" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="L107" s="25"/>
       <c r="M107" s="25"/>
@@ -15043,7 +15076,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>L104:M107 J104:J107 O104:O107 O69:O81 J25:J81 O10:O20 O22:O23 L22:M23 J22:J23 J10:J20 L10:M20 O25:O67 L25:M67 L69:M81</xm:sqref>
+          <xm:sqref>L104:M107 J104:J107 O104:O107 J25:J81 O10:O20 O22:O23 L22:M23 J22:J23 J10:J20 L10:M20 O25:O81 L25:M81</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>

</xml_diff>